<commit_message>
Szótár abc sorrendben, mert fogyatékos vagyok és elfejeltettem :)
</commit_message>
<xml_diff>
--- a/kaposvari_szotar_2.5.xlsx
+++ b/kaposvari_szotar_2.5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaposvarigergo/Desktop/projlab/projlabcsinibaba/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E126052-07A2-CA48-A26E-D0D9BDC9867D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC14879-E0FF-C648-9B06-51A93D100AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17160" xr2:uid="{9D6DDD07-AD74-BB4E-9AC5-E8A1A4655CB9}"/>
   </bookViews>
@@ -567,42 +567,42 @@
   <sheetData>
     <row r="2" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19" x14ac:dyDescent="0.25">
@@ -615,106 +615,106 @@
     </row>
     <row r="8" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>39</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="19" x14ac:dyDescent="0.25">
@@ -727,53 +727,56 @@
     </row>
     <row r="22" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B27">
+    <sortCondition ref="A1:A27"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>